<commit_message>
Added email field and some other changes(see below): 1. Few docs fixes 2. Fixed unexpected crashing while attempting to generate fee receipt from utilities section 3. Added backend for sending notification mail depending upon filters applied
</commit_message>
<xml_diff>
--- a/src/demo_student.xlsx
+++ b/src/demo_student.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="106">
   <si>
     <t xml:space="preserve">Roll no.</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Willie M. Vargas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcdef@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">39/CSE/17002</t>
@@ -344,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -366,6 +369,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -410,8 +419,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,18 +453,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:D224"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -471,555 +488,708 @@
       <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>200</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>201</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>202</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>203</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>204</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>205</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>206</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>207</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>208</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>209</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>210</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>211</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>212</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>213</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>214</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>215</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>216</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>217</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>218</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>219</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>220</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>221</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>222</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>223</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>224</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>225</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>226</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>227</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>228</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>229</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>230</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>231</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>232</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>233</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>234</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>235</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>236</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>237</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>238</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>239</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>240</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>241</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>242</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>243</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>244</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>245</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>246</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>247</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>248</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>249</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1050,7 +1220,7 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="1"/>
+      <c r="C80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1104,7 +1274,7 @@
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="1"/>
+      <c r="C132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1199,6 +1369,59 @@
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="abcdef@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="abcdef@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="abcdef@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="abcdef@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="abcdef@gmail.com"/>
+    <hyperlink ref="D7" r:id="rId6" display="abcdef@gmail.com"/>
+    <hyperlink ref="D8" r:id="rId7" display="abcdef@gmail.com"/>
+    <hyperlink ref="D9" r:id="rId8" display="abcdef@gmail.com"/>
+    <hyperlink ref="D10" r:id="rId9" display="abcdef@gmail.com"/>
+    <hyperlink ref="D11" r:id="rId10" display="abcdef@gmail.com"/>
+    <hyperlink ref="D12" r:id="rId11" display="abcdef@gmail.com"/>
+    <hyperlink ref="D13" r:id="rId12" display="abcdef@gmail.com"/>
+    <hyperlink ref="D14" r:id="rId13" display="abcdef@gmail.com"/>
+    <hyperlink ref="D15" r:id="rId14" display="abcdef@gmail.com"/>
+    <hyperlink ref="D16" r:id="rId15" display="abcdef@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId16" display="abcdef@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId17" display="abcdef@gmail.com"/>
+    <hyperlink ref="D19" r:id="rId18" display="abcdef@gmail.com"/>
+    <hyperlink ref="D20" r:id="rId19" display="abcdef@gmail.com"/>
+    <hyperlink ref="D21" r:id="rId20" display="abcdef@gmail.com"/>
+    <hyperlink ref="D22" r:id="rId21" display="abcdef@gmail.com"/>
+    <hyperlink ref="D23" r:id="rId22" display="abcdef@gmail.com"/>
+    <hyperlink ref="D24" r:id="rId23" display="abcdef@gmail.com"/>
+    <hyperlink ref="D25" r:id="rId24" display="abcdef@gmail.com"/>
+    <hyperlink ref="D26" r:id="rId25" display="abcdef@gmail.com"/>
+    <hyperlink ref="D27" r:id="rId26" display="abcdef@gmail.com"/>
+    <hyperlink ref="D28" r:id="rId27" display="abcdef@gmail.com"/>
+    <hyperlink ref="D29" r:id="rId28" display="abcdef@gmail.com"/>
+    <hyperlink ref="D30" r:id="rId29" display="abcdef@gmail.com"/>
+    <hyperlink ref="D31" r:id="rId30" display="abcdef@gmail.com"/>
+    <hyperlink ref="D32" r:id="rId31" display="abcdef@gmail.com"/>
+    <hyperlink ref="D33" r:id="rId32" display="abcdef@gmail.com"/>
+    <hyperlink ref="D34" r:id="rId33" display="abcdef@gmail.com"/>
+    <hyperlink ref="D35" r:id="rId34" display="abcdef@gmail.com"/>
+    <hyperlink ref="D36" r:id="rId35" display="abcdef@gmail.com"/>
+    <hyperlink ref="D37" r:id="rId36" display="abcdef@gmail.com"/>
+    <hyperlink ref="D38" r:id="rId37" display="abcdef@gmail.com"/>
+    <hyperlink ref="D39" r:id="rId38" display="abcdef@gmail.com"/>
+    <hyperlink ref="D40" r:id="rId39" display="abcdef@gmail.com"/>
+    <hyperlink ref="D41" r:id="rId40" display="abcdef@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId41" display="abcdef@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId42" display="abcdef@gmail.com"/>
+    <hyperlink ref="D44" r:id="rId43" display="abcdef@gmail.com"/>
+    <hyperlink ref="D45" r:id="rId44" display="abcdef@gmail.com"/>
+    <hyperlink ref="D46" r:id="rId45" display="abcdef@gmail.com"/>
+    <hyperlink ref="D47" r:id="rId46" display="abcdef@gmail.com"/>
+    <hyperlink ref="D48" r:id="rId47" display="abcdef@gmail.com"/>
+    <hyperlink ref="D49" r:id="rId48" display="abcdef@gmail.com"/>
+    <hyperlink ref="D50" r:id="rId49" display="abcdef@gmail.com"/>
+    <hyperlink ref="D51" r:id="rId50" display="abcdef@gmail.com"/>
+    <hyperlink ref="D52" r:id="rId51" display="abcdef@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>